<commit_message>
added files for multiple i to be able to work on that calmly
</commit_message>
<xml_diff>
--- a/R_bachelorarbeit/data_fitting/merged_impfdaten.xlsx
+++ b/R_bachelorarbeit/data_fitting/merged_impfdaten.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dokumente\Uni\TUM\Mathe_B_Sc\SS_20\Bachelorarbeit\bachelorarbeit-repo\R_bachelorarbeit\data_fitting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D45B53E0-76BE-4924-AAFF-A1D215479095}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C37353-3F5B-45EC-AB34-B4C938AE703D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3735" yWindow="3945" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1702,8 +1702,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L414"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A388" workbookViewId="0">
-      <selection activeCell="E402" sqref="E402:F414"/>
+    <sheetView tabSelected="1" topLeftCell="A379" workbookViewId="0">
+      <selection activeCell="K402" sqref="K402:K414"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1790,10 +1790,6 @@
       <c r="F3" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K66" si="0">H3/$L$2</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -1821,7 +1817,7 @@
         <v>1</v>
       </c>
       <c r="K4">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="K3:K66" si="0">H4/$L$2</f>
         <v>2.8900000000000002E-2</v>
       </c>
     </row>
@@ -1874,10 +1870,6 @@
       <c r="F6" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1898,10 +1890,6 @@
       <c r="F7" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -2132,10 +2120,6 @@
       <c r="F15" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K15">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -2156,10 +2140,6 @@
       <c r="F16" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -2210,10 +2190,6 @@
       <c r="F18" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -2324,10 +2300,6 @@
       <c r="F22" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K22">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -2348,10 +2320,6 @@
       <c r="F23" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K23">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -2462,10 +2430,6 @@
       <c r="F27" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
@@ -2486,10 +2450,6 @@
       <c r="F28" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
@@ -2660,10 +2620,6 @@
       <c r="F34" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K34">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
@@ -2714,10 +2670,6 @@
       <c r="F36" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -2738,10 +2690,6 @@
       <c r="F37" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
@@ -3062,10 +3010,6 @@
       <c r="F48" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K48">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
@@ -3206,10 +3150,6 @@
       <c r="F53" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K53">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
@@ -3290,10 +3230,6 @@
       <c r="F56" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K56">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
@@ -3344,10 +3280,6 @@
       <c r="F58" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
@@ -3398,10 +3330,6 @@
       <c r="F60" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K60">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
@@ -3572,10 +3500,6 @@
       <c r="F66" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K66">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
@@ -3656,10 +3580,6 @@
       <c r="F69" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K69">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
@@ -3680,10 +3600,6 @@
       <c r="F70" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K70">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
@@ -3764,10 +3680,6 @@
       <c r="F73" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K73">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
@@ -3788,10 +3700,6 @@
       <c r="F74" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K74">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
@@ -3842,10 +3750,6 @@
       <c r="F76" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K76">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
@@ -3896,10 +3800,6 @@
       <c r="F78" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K78">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
@@ -3980,10 +3880,6 @@
       <c r="F81" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K81">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
@@ -4004,10 +3900,6 @@
       <c r="F82" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K82">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
@@ -4028,10 +3920,6 @@
       <c r="F83" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K83">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
@@ -4142,10 +4030,6 @@
       <c r="F87" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K87">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
@@ -4196,10 +4080,6 @@
       <c r="F89" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K89">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
@@ -4250,10 +4130,6 @@
       <c r="F91" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K91">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
@@ -4334,10 +4210,6 @@
       <c r="F94" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K94">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
@@ -4388,10 +4260,6 @@
       <c r="F96" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K96">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
@@ -4592,10 +4460,6 @@
       <c r="F103" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K103">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
@@ -4856,10 +4720,6 @@
       <c r="F112" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K112">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
@@ -4880,10 +4740,6 @@
       <c r="F113" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K113">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
@@ -4904,10 +4760,6 @@
       <c r="F114" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K114">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
@@ -4958,10 +4810,6 @@
       <c r="F116" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K116">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
@@ -5012,10 +4860,6 @@
       <c r="F118" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K118">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
@@ -5126,10 +4970,6 @@
       <c r="F122" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K122">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
@@ -5210,10 +5050,6 @@
       <c r="F125" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K125">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
@@ -5234,10 +5070,6 @@
       <c r="F126" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K126">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
@@ -5318,10 +5150,6 @@
       <c r="F129" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K129">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
@@ -5342,10 +5170,6 @@
       <c r="F130" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K130">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
@@ -5486,10 +5310,6 @@
       <c r="F135" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K135">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
@@ -5540,10 +5360,6 @@
       <c r="F137" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K137">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
@@ -5594,10 +5410,6 @@
       <c r="F139" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K139">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
@@ -5888,10 +5700,6 @@
       <c r="F149" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K149">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
@@ -5912,10 +5720,6 @@
       <c r="F150" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K150">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
@@ -5936,10 +5740,6 @@
       <c r="F151" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K151">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
@@ -6140,10 +5940,6 @@
       <c r="F158" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K158">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
@@ -6224,10 +6020,6 @@
       <c r="F161" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K161">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
@@ -6368,10 +6160,6 @@
       <c r="F166" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K166">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
@@ -6512,10 +6300,6 @@
       <c r="F171" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K171">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
@@ -6566,10 +6350,6 @@
       <c r="F173" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K173">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
@@ -6590,10 +6370,6 @@
       <c r="F174" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K174">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
@@ -6644,10 +6420,6 @@
       <c r="F176" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K176">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
@@ -6698,10 +6470,6 @@
       <c r="F178" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K178">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
@@ -6722,10 +6490,6 @@
       <c r="F179" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K179">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
@@ -6776,10 +6540,6 @@
       <c r="F181" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K181">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
@@ -6830,10 +6590,6 @@
       <c r="F183" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K183">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
@@ -6884,10 +6640,6 @@
       <c r="F185" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K185">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
@@ -6908,10 +6660,6 @@
       <c r="F186" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K186">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
@@ -7022,10 +6770,6 @@
       <c r="F190" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K190">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
@@ -7076,10 +6820,6 @@
       <c r="F192" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K192">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
@@ -7190,10 +6930,6 @@
       <c r="F196" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K196">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
@@ -7244,10 +6980,6 @@
       <c r="F198" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K198">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
@@ -7298,10 +7030,6 @@
       <c r="F200" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K200">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
@@ -7352,10 +7080,6 @@
       <c r="F202" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K202">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
@@ -7406,10 +7130,6 @@
       <c r="F204" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K204">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
@@ -7460,10 +7180,6 @@
       <c r="F206" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K206">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
@@ -7694,10 +7410,6 @@
       <c r="F214" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K214">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
@@ -7838,10 +7550,6 @@
       <c r="F219" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K219">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
@@ -7952,10 +7660,6 @@
       <c r="F223" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K223">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
@@ -8006,10 +7710,6 @@
       <c r="F225" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K225">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
@@ -8030,10 +7730,6 @@
       <c r="F226" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K226">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
@@ -8084,10 +7780,6 @@
       <c r="F228" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K228">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
@@ -8168,10 +7860,6 @@
       <c r="F231" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K231">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
@@ -8282,10 +7970,6 @@
       <c r="F235" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K235">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
@@ -8486,10 +8170,6 @@
       <c r="F242" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K242">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="243" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
@@ -8780,10 +8460,6 @@
       <c r="F252" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K252">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="253" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
@@ -8834,10 +8510,6 @@
       <c r="F254" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K254">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="255" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
@@ -8918,10 +8590,6 @@
       <c r="F257" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K257">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="258" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
@@ -9062,10 +8730,6 @@
       <c r="F262" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K262">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="263" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
@@ -9086,10 +8750,6 @@
       <c r="F263" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K263">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="264" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
@@ -9170,10 +8830,6 @@
       <c r="F266" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K266">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="267" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
@@ -9254,10 +8910,6 @@
       <c r="F269" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K269">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="270" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
@@ -9308,10 +8960,6 @@
       <c r="F271" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K271">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="272" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
@@ -9452,10 +9100,6 @@
       <c r="F276" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K276">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="277" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
@@ -9506,10 +9150,6 @@
       <c r="F278" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K278">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="279" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
@@ -9530,10 +9170,6 @@
       <c r="F279" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K279">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="280" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
@@ -9614,10 +9250,6 @@
       <c r="F282" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K282">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="283" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
@@ -9638,10 +9270,6 @@
       <c r="F283" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K283">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="284" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
@@ -9662,10 +9290,6 @@
       <c r="F284" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K284">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="285" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
@@ -9806,10 +9430,6 @@
       <c r="F289" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K289">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="290" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
@@ -9890,10 +9510,6 @@
       <c r="F292" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K292">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="293" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
@@ -10064,10 +9680,6 @@
       <c r="F298" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K298">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="299" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
@@ -10088,10 +9700,6 @@
       <c r="F299" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K299">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="300" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
@@ -10472,10 +10080,6 @@
       <c r="F312" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K312">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="313" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
@@ -10496,10 +10100,6 @@
       <c r="F313" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K313">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="314" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
@@ -10550,10 +10150,6 @@
       <c r="F315" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K315">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="316" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
@@ -10664,10 +10260,6 @@
       <c r="F319" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K319">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="320" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
@@ -10778,10 +10370,6 @@
       <c r="F323" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K323">
-        <f t="shared" ref="K323:K386" si="5">H323/$L$2</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="324" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
@@ -10809,7 +10397,7 @@
         <v>12</v>
       </c>
       <c r="K324">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="K323:K386" si="5">H324/$L$2</f>
         <v>2.1499999999999998E-2</v>
       </c>
     </row>
@@ -10862,10 +10450,6 @@
       <c r="F326" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K326">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="327" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
@@ -10886,10 +10470,6 @@
       <c r="F327" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K327">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="328" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
@@ -10910,10 +10490,6 @@
       <c r="F328" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K328">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="329" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
@@ -11024,10 +10600,6 @@
       <c r="F332" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K332">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="333" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
@@ -11138,10 +10710,6 @@
       <c r="F336" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K336">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="337" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
@@ -11162,10 +10730,6 @@
       <c r="F337" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K337">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="338" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
@@ -11186,10 +10750,6 @@
       <c r="F338" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K338">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="339" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
@@ -11210,10 +10770,6 @@
       <c r="F339" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K339">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="340" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
@@ -11354,10 +10910,6 @@
       <c r="F344" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K344">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="345" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
@@ -11408,10 +10960,6 @@
       <c r="F346" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K346">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="347" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
@@ -11432,10 +10980,6 @@
       <c r="F347" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K347">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="348" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
@@ -11456,10 +11000,6 @@
       <c r="F348" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K348">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="349" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
@@ -11480,10 +11020,6 @@
       <c r="F349" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K349">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="350" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
@@ -11594,10 +11130,6 @@
       <c r="F353" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K353">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="354" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
@@ -11918,10 +11450,6 @@
       <c r="F364" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K364">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="365" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
@@ -12032,10 +11560,6 @@
       <c r="F368" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K368">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="369" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
@@ -12146,10 +11670,6 @@
       <c r="F372" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K372">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="373" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
@@ -12170,10 +11690,6 @@
       <c r="F373" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K373">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="374" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
@@ -12254,10 +11770,6 @@
       <c r="F376" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K376">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="377" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
@@ -12278,10 +11790,6 @@
       <c r="F377" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K377">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="378" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
@@ -12302,10 +11810,6 @@
       <c r="F378" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K378">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="379" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
@@ -12326,10 +11830,6 @@
       <c r="F379" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K379">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="380" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
@@ -12380,10 +11880,6 @@
       <c r="F381" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K381">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="382" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
@@ -12494,10 +11990,6 @@
       <c r="F385" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K385">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="386" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
@@ -12818,10 +12310,6 @@
       <c r="F396" s="1">
         <v>80.180000000000007</v>
       </c>
-      <c r="K396">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="397" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
@@ -12992,10 +12480,6 @@
       <c r="F402" t="s">
         <v>443</v>
       </c>
-      <c r="K402">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="403" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
@@ -13016,10 +12500,6 @@
       <c r="F403" t="s">
         <v>443</v>
       </c>
-      <c r="K403">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="404" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
@@ -13040,10 +12520,6 @@
       <c r="F404" t="s">
         <v>443</v>
       </c>
-      <c r="K404">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="405" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
@@ -13064,10 +12540,6 @@
       <c r="F405" t="s">
         <v>443</v>
       </c>
-      <c r="K405">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="406" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
@@ -13088,10 +12560,6 @@
       <c r="F406" t="s">
         <v>443</v>
       </c>
-      <c r="K406">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="407" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
@@ -13112,10 +12580,6 @@
       <c r="F407" t="s">
         <v>443</v>
       </c>
-      <c r="K407">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="408" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
@@ -13136,10 +12600,6 @@
       <c r="F408" t="s">
         <v>443</v>
       </c>
-      <c r="K408">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="409" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
@@ -13160,10 +12620,6 @@
       <c r="F409" t="s">
         <v>443</v>
       </c>
-      <c r="K409">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="410" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
@@ -13184,10 +12640,6 @@
       <c r="F410" t="s">
         <v>443</v>
       </c>
-      <c r="K410">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="411" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
@@ -13208,10 +12660,6 @@
       <c r="F411" t="s">
         <v>443</v>
       </c>
-      <c r="K411">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="412" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
@@ -13232,10 +12680,6 @@
       <c r="F412" t="s">
         <v>443</v>
       </c>
-      <c r="K412">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="413" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
@@ -13256,10 +12700,6 @@
       <c r="F413" t="s">
         <v>443</v>
       </c>
-      <c r="K413">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="414" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
@@ -13279,10 +12719,6 @@
       </c>
       <c r="F414" t="s">
         <v>443</v>
-      </c>
-      <c r="K414">
-        <f t="shared" si="6"/>
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>